<commit_message>
updated testdata and ReportsConfig
</commit_message>
<xml_diff>
--- a/src/test/resources/com/google/excel/testdata.xlsx
+++ b/src/test/resources/com/google/excel/testdata.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HarishVITO\Desktop\KCSA3\PageObjectModelBasics\src\test\resources\com\google\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D6A11D-B053-4E05-A593-7E81E2B2F956}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C110F078-6F16-489E-9486-DCBDAA8FF14D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="20760" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -18,6 +13,7 @@
     <sheet name="CreateAccountTest" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:L8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,9 +43,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>harishch548@gmail.com</t>
-  </si>
-  <si>
     <t>loveisdamngood</t>
   </si>
   <si>
@@ -60,6 +53,9 @@
   </si>
   <si>
     <t>Harish</t>
+  </si>
+  <si>
+    <t>harishvito@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -417,7 +413,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -432,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,10 +452,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -477,7 +473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8A6C51-73E5-42C5-9137-FE60D23F5498}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -488,12 +484,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>